<commit_message>
remove hyperlinks on the urls
</commit_message>
<xml_diff>
--- a/papers-in-sessions.xlsx
+++ b/papers-in-sessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Projects/acs2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C177F719-A1A6-2C40-9920-99A94416F07C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704C3819-4523-BF4E-823D-54E352E49225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15020" yWindow="5240" windowWidth="33120" windowHeight="21260" xr2:uid="{C59E5D1B-900F-9745-BB9B-F644F9F51CF1}"/>
   </bookViews>
@@ -329,7 +329,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +339,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -416,9 +423,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -443,8 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,7 +769,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,7 +921,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -928,7 +934,7 @@
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1013,7 +1019,7 @@
       <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1187,7 +1193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1200,11 +1206,11 @@
       <c r="D25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1217,7 +1223,7 @@
       <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1234,7 +1240,7 @@
       <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1272,7 +1278,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>33</v>
       </c>
@@ -1285,7 +1291,7 @@
       <c r="D30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1326,13 +1332,6 @@
   <sortState ref="A2:D31">
     <sortCondition ref="A2:A31"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{A8CCEEBC-797A-EC4C-9E30-581089DADC04}"/>
-    <hyperlink ref="E25" r:id="rId2" xr:uid="{C1A93B85-77C0-5C46-965B-42C2F6A5BC8C}"/>
-    <hyperlink ref="E26" r:id="rId3" xr:uid="{F2BA5AD2-C94D-CF4E-B5DF-BE6DDE50DE8B}"/>
-    <hyperlink ref="E27" r:id="rId4" xr:uid="{92AC92FB-1D87-9D47-B2FC-9CA525F58A91}"/>
-    <hyperlink ref="E30" r:id="rId5" xr:uid="{27EB3973-60A1-A240-947F-FBF235F33648}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
forgot to push this.
</commit_message>
<xml_diff>
--- a/papers-in-sessions.xlsx
+++ b/papers-in-sessions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Projects/acs2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EF411D6-2F14-C841-A8CE-134742F63148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D988AF09-181A-FB4F-87EF-2DFFB4188A3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="6460" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="16900" yWindow="5560" windowWidth="22900" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="papers-in-sessions" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1313,7 +1313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
@@ -1323,7 +1323,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="45.33203125" customWidth="1"/>
-    <col min="7" max="7" width="64.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>